<commit_message>
finialise docs for submition for sprint 2
</commit_message>
<xml_diff>
--- a/docs/ProjectBackLog.xlsx
+++ b/docs/ProjectBackLog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\capstone\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{90D11B97-B9ED-491F-8D34-6EAD2827E6DB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95CF876-4212-4F40-8A3F-62F4E7B8E2C7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C1B21EA-7C3A-473C-B0DC-143A97C8C0BF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>Task</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>As a Coach I want to be able to view the boat moving on a map so I can track our position on a boat during practice to help our performance</t>
+  </si>
+  <si>
+    <t>Priority</t>
   </si>
 </sst>
 </file>
@@ -192,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -201,13 +204,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <alignment vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -237,14 +249,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E8E2312-6998-4028-AC26-93C50242B906}" name="Table1" displayName="Table1" ref="A1:E29" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:E29" xr:uid="{2F9CF247-493B-4E4B-9879-8DBD76422874}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E8E2312-6998-4028-AC26-93C50242B906}" name="Table1" displayName="Table1" ref="A1:F29" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:F29" xr:uid="{2F9CF247-493B-4E4B-9879-8DBD76422874}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{1C0F70AE-6B56-486D-87EB-958F1C1DF572}" name="ID" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{90A8BCD8-DCDB-4461-8F25-70A55E6F852D}" name="Task" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{FDA24D50-4AF9-4CE5-BCF7-C106CC20CFF3}" name="Story" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{81DB1257-C1C5-417C-A6CC-B7D8068EF3D0}" name="Story Points"/>
     <tableColumn id="5" xr3:uid="{5006F6C9-42ED-4D65-9C09-EAE3C6EF3EBE}" name="Estimation(Days)"/>
+    <tableColumn id="6" xr3:uid="{ED408448-7152-4EFC-A450-A0E8AEFB8D55}" name="Priority"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -509,28 +522,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30CCA17D-4044-4E1C-9B3F-ADC041FF8CEA}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="35.25" customWidth="1"/>
-    <col min="3" max="3" width="121.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="79.25" style="6" customWidth="1"/>
     <col min="4" max="4" width="13.125" customWidth="1"/>
     <col min="5" max="5" width="17.375" customWidth="1"/>
+    <col min="6" max="6" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -539,15 +553,18 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D2">
@@ -556,180 +573,216 @@
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="4"/>
       <c r="D3">
         <v>10</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="4"/>
       <c r="D4">
         <v>15</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="4"/>
       <c r="D5">
         <v>5</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="4"/>
       <c r="D6">
         <v>15</v>
       </c>
       <c r="E6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="4"/>
       <c r="D7">
         <v>15</v>
       </c>
       <c r="E7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="4"/>
       <c r="D8">
         <v>10</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="4"/>
       <c r="D9">
         <v>5</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="4"/>
       <c r="D10">
         <v>15</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="4"/>
       <c r="D11">
         <v>15</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="4"/>
       <c r="D12">
         <v>5</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="4"/>
       <c r="D13">
         <v>10</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D14">
@@ -738,15 +791,18 @@
       <c r="E14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D15">
@@ -755,30 +811,36 @@
       <c r="E15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="4"/>
       <c r="D16">
         <v>10</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D17">
@@ -787,30 +849,36 @@
       <c r="E17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="3"/>
+      <c r="C18" s="4"/>
       <c r="D18">
         <v>5</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D19">
@@ -819,15 +887,18 @@
       <c r="E19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D20">
@@ -836,15 +907,18 @@
       <c r="E20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D21">
@@ -853,15 +927,18 @@
       <c r="E21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D22">
@@ -870,15 +947,18 @@
       <c r="E22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D23">
@@ -887,15 +967,18 @@
       <c r="E23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D24">
@@ -904,45 +987,54 @@
       <c r="E24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="3"/>
+      <c r="C25" s="4"/>
       <c r="D25">
         <v>15</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="3"/>
+      <c r="C26" s="4"/>
       <c r="D26">
         <v>5</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D27">
@@ -951,15 +1043,18 @@
       <c r="E27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D28">
@@ -968,15 +1063,18 @@
       <c r="E28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D29">
@@ -984,6 +1082,9 @@
       </c>
       <c r="E29">
         <v>1</v>
+      </c>
+      <c r="F29">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>